<commit_message>
Colorado Avalanche have won the Stanley Cup!!!
Updating file for the new 2022 Stanley Cup Champions, the Colorado Avalanche!
</commit_message>
<xml_diff>
--- a/NHL_Champions.xlsx
+++ b/NHL_Champions.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,7 +449,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Data as of  06.26.2022 01:55 AM</t>
+          <t>Data as of  06.28.2022 01:54 AM</t>
         </is>
       </c>
     </row>
@@ -472,22 +472,22 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tampa Bay Lightning</t>
+          <t>Colorado Avalanche</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Coach Jon Cooper</t>
+          <t>Coach Jared Bednar</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -502,52 +502,52 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>St. Louis Blues</t>
+          <t>Tampa Bay Lightning</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Coach Craig Berube</t>
+          <t>Coach Jon Cooper</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Washington Capitals</t>
+          <t>St. Louis Blues</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Coach Barry Trotz</t>
+          <t>Coach Craig Berube</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Pittsburgh Penguins</t>
+          <t>Washington Capitals</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Coach Mike Sullivan</t>
+          <t>Coach Barry Trotz</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -562,262 +562,262 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Chicago Blackhawks</t>
+          <t>Pittsburgh Penguins</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Coach Joel Quenneville</t>
+          <t>Coach Mike Sullivan</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Los Angeles Kings</t>
+          <t>Chicago Blackhawks</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Coach Darryl Sutter</t>
+          <t>Coach Joel Quenneville</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Chicago Blackhawks</t>
+          <t>Los Angeles Kings</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Coach Joel Quenneville</t>
+          <t>Coach Darryl Sutter</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Los Angeles Kings</t>
+          <t>Chicago Blackhawks</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Coach Darryl Sutter</t>
+          <t>Coach Joel Quenneville</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Boston Bruins</t>
+          <t>Los Angeles Kings</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Coach Claude Julien</t>
+          <t>Coach Darryl Sutter</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Chicago Blackhawks</t>
+          <t>Boston Bruins</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Coach Joel Quenneville</t>
+          <t>Coach Claude Julien</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Pittsburgh Penguins</t>
+          <t>Chicago Blackhawks</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Coach Dan Bylsma</t>
+          <t>Coach Joel Quenneville</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Detroit Red Wings</t>
+          <t>Pittsburgh Penguins</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Coach Mike Babcock</t>
+          <t>Coach Dan Bylsma</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Anaheim Ducks</t>
+          <t>Detroit Red Wings</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve">Coach Randy Carlyle </t>
+          <t>Coach Mike Babcock</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Carolina Hurricanes</t>
+          <t>Anaheim Ducks</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Coach Peter Laviolette</t>
+          <t xml:space="preserve">Coach Randy Carlyle </t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Tampa Bay Lightning</t>
+          <t>Carolina Hurricanes</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Coach John Tortorella</t>
+          <t>Coach Peter Laviolette</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>New Jersey Devils</t>
+          <t>Tampa Bay Lightning</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Coach Pat Burns</t>
+          <t>Coach John Tortorella</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Detroit Red Wings</t>
+          <t>New Jersey Devils</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Coach Scotty Bowman</t>
+          <t>Coach Pat Burns</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Colorado Avalanche</t>
+          <t>Detroit Red Wings</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Coach Bob Hartley</t>
+          <t>Coach Scotty Bowman</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>New Jersey Devils</t>
+          <t>Colorado Avalanche</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Coach Larry Robinson</t>
+          <t>Coach Bob Hartley</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Dallas Stars</t>
+          <t>New Jersey Devils</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Coach Ken Hitchcock</t>
+          <t>Coach Larry Robinson</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Detroit Red Wings</t>
+          <t>Dallas Stars</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Coach Scotty Bowman</t>
+          <t>Coach Ken Hitchcock</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -832,82 +832,82 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Colorado Avalanche</t>
+          <t>Detroit Red Wings</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Coach Marc Crawford</t>
+          <t>Coach Scotty Bowman</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>New Jersey Devils</t>
+          <t>Colorado Avalanche</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Coach Jacques Lemaire</t>
+          <t>Coach Marc Crawford</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>New York Rangers</t>
+          <t>New Jersey Devils</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Coach Mike Keenan</t>
+          <t>Coach Jacques Lemaire</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Montreal Canadiens</t>
+          <t>New York Rangers</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Coach Jacques Demers</t>
+          <t>Coach Mike Keenan</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Pittsburgh Penguins</t>
+          <t>Montreal Canadiens</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Coach Scotty Bowman</t>
+          <t>Coach Jacques Demers</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -916,58 +916,58 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Coach Bob Johnson</t>
+          <t>Coach Scotty Bowman</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Edmonton Oilers</t>
+          <t>Pittsburgh Penguins</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Coach John Muckler</t>
+          <t>Coach Bob Johnson</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Calgary Flames</t>
+          <t>Edmonton Oilers</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Coach Terry Crisp</t>
+          <t>Coach John Muckler</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Edmonton Oilers</t>
+          <t>Calgary Flames</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Coach Glen Sather</t>
+          <t>Coach Terry Crisp</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -982,37 +982,37 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Montreal Canadiens</t>
+          <t>Edmonton Oilers</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Coach Jean Perron</t>
+          <t>Coach Glen Sather</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Edmonton Oilers</t>
+          <t>Montreal Canadiens</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Coach Glen Sather</t>
+          <t>Coach Jean Perron</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1027,22 +1027,22 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>New York Islanders</t>
+          <t>Edmonton Oilers</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Coach Al Arbour</t>
+          <t>Coach Glen Sather</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1981</v>
+        <v>1982</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1087,22 +1087,22 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1979</v>
+        <v>1980</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Montreal Canadiens</t>
+          <t>New York Islanders</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Coach Scotty Bowman</t>
+          <t>Coach Al Arbour</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1978</v>
+        <v>1979</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -1117,7 +1117,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1976</v>
+        <v>1977</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1147,22 +1147,22 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1975</v>
+        <v>1976</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Philadelphia Flyers</t>
+          <t>Montreal Canadiens</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Coach Fred Shero</t>
+          <t>Coach Scotty Bowman</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1974</v>
+        <v>1975</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -1177,82 +1177,82 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1973</v>
+        <v>1974</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Montreal Canadiens</t>
+          <t>Philadelphia Flyers</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Coach Scotty Bowman</t>
+          <t>Coach Fred Shero</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1972</v>
+        <v>1973</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Boston Bruins</t>
+          <t>Montreal Canadiens</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Coach Tom Johnson</t>
+          <t>Coach Scotty Bowman</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Montreal Canadiens</t>
+          <t>Boston Bruins</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Coach Al MacNeil</t>
+          <t>Coach Tom Johnson</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1970</v>
+        <v>1971</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Boston Bruins</t>
+          <t>Montreal Canadiens</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Coach Harry Sinden</t>
+          <t>Coach Al MacNeil</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Montreal Canadiens</t>
+          <t>Boston Bruins</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Coach Claude Ruel</t>
+          <t>Coach Harry Sinden</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1968</v>
+        <v>1969</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -1261,43 +1261,43 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Coach Toe Blake</t>
+          <t>Coach Claude Ruel</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1967</v>
+        <v>1968</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Toronto Maple Leafs</t>
+          <t>Montreal Canadiens</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Coach Punch Imlach</t>
+          <t>Coach Toe Blake</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1966</v>
+        <v>1967</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Montreal Canadiens</t>
+          <t>Toronto Maple Leafs</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Coach Toe Blake</t>
+          <t>Coach Punch Imlach</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1965</v>
+        <v>1966</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -1312,22 +1312,22 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1964</v>
+        <v>1965</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Toronto Maple Leafs</t>
+          <t>Montreal Canadiens</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Coach Punch Imlach</t>
+          <t>Coach Toe Blake</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1963</v>
+        <v>1964</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -1342,7 +1342,7 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1962</v>
+        <v>1963</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -1357,37 +1357,37 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1961</v>
+        <v>1962</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Chicago Black Hawks</t>
+          <t>Toronto Maple Leafs</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Coach Rudy Pilous</t>
+          <t>Coach Punch Imlach</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Montreal Canadiens</t>
+          <t>Chicago Black Hawks</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Coach Toe Blake</t>
+          <t>Coach Rudy Pilous</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>1959</v>
+        <v>1960</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>1958</v>
+        <v>1959</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1957</v>
+        <v>1958</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>1956</v>
+        <v>1957</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -1447,22 +1447,22 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1955</v>
+        <v>1956</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Detroit Red Wings</t>
+          <t>Montreal Canadiens</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Coach Jimmy Skinner</t>
+          <t>Coach Toe Blake</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>1954</v>
+        <v>1955</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -1471,88 +1471,88 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Coach Tommy Ivan</t>
+          <t>Coach Jimmy Skinner</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>1953</v>
+        <v>1954</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Montreal Canadiens</t>
+          <t>Detroit Red Wings</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Coach Dick Irvin</t>
+          <t>Coach Tommy Ivan</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>1952</v>
+        <v>1953</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Detroit Red Wings</t>
+          <t>Montreal Canadiens</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Coach Tommy Ivan</t>
+          <t>Coach Dick Irvin</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>1951</v>
+        <v>1952</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Toronto Maple Leafs</t>
+          <t>Detroit Red Wings</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Coach Joe Primeau</t>
+          <t>Coach Tommy Ivan</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>1950</v>
+        <v>1951</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Detroit Red Wings</t>
+          <t>Toronto Maple Leafs</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Coach Tommy Ivan</t>
+          <t>Coach Joe Primeau</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>1949</v>
+        <v>1950</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Toronto Maple Leafs</t>
+          <t>Detroit Red Wings</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Coach Hap Day</t>
+          <t>Coach Tommy Ivan</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1948</v>
+        <v>1949</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>1947</v>
+        <v>1948</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -1582,157 +1582,157 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>1946</v>
+        <v>1947</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Montreal Canadiens</t>
+          <t>Toronto Maple Leafs</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Coach Dick Irvin</t>
+          <t>Coach Hap Day</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>1945</v>
+        <v>1946</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Toronto Maple Leafs</t>
+          <t>Montreal Canadiens</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Coach Hap Day</t>
+          <t>Coach Dick Irvin</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>1944</v>
+        <v>1945</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Montreal Canadiens</t>
+          <t>Toronto Maple Leafs</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Coach Dick Irvin</t>
+          <t>Coach Hap Day</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>1943</v>
+        <v>1944</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Detroit Red Wings</t>
+          <t>Montreal Canadiens</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Coach Jack Adams</t>
+          <t>Coach Dick Irvin</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>1942</v>
+        <v>1943</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Toronto Maple Leafs</t>
+          <t>Detroit Red Wings</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Coach Hap Day</t>
+          <t>Coach Jack Adams</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>1941</v>
+        <v>1942</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Boston Bruins</t>
+          <t>Toronto Maple Leafs</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Coach Cooney Weiland</t>
+          <t>Coach Hap Day</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>1940</v>
+        <v>1941</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>New York Rangers</t>
+          <t>Boston Bruins</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Coach Frank Boucher</t>
+          <t>Coach Cooney Weiland</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1939</v>
+        <v>1940</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Boston Bruins</t>
+          <t>New York Rangers</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Coach Art Ross</t>
+          <t>Coach Frank Boucher</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1938</v>
+        <v>1939</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Chicago Black Hawks</t>
+          <t>Boston Bruins</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Coach Bill Stewart</t>
+          <t>Coach Art Ross</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>1937</v>
+        <v>1938</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Detroit Red Wings</t>
+          <t>Chicago Black Hawks</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Coach Jack Adams</t>
+          <t>Coach Bill Stewart</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>1936</v>
+        <v>1937</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -1747,26 +1747,26 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>1935</v>
+        <v>1936</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Montreal Maroons</t>
+          <t>Detroit Red Wings</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Coach Tommy Gorman</t>
+          <t>Coach Jack Adams</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Chicago Black Hawks</t>
+          <t>Montreal Maroons</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -1777,52 +1777,52 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>New York Rangers</t>
+          <t>Chicago Black Hawks</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Coach Lester Patrick</t>
+          <t>Coach Tommy Gorman</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>1932</v>
+        <v>1933</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Toronto Maple Leafs</t>
+          <t>New York Rangers</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Coach Dick Irvin</t>
+          <t>Coach Lester Patrick</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Montreal Canadiens</t>
+          <t>Toronto Maple Leafs</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Coach Cecil Hart</t>
+          <t>Coach Dick Irvin</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>1930</v>
+        <v>1931</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -1837,44 +1837,59 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>1929</v>
+        <v>1930</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Boston Bruins</t>
+          <t>Montreal Canadiens</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Coach Cy Denneny</t>
+          <t>Coach Cecil Hart</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>1928</v>
+        <v>1929</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>New York Rangers</t>
+          <t>Boston Bruins</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Coach Lester Patrick</t>
+          <t>Coach Cy Denneny</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
+        <v>1928</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>New York Rangers</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Coach Lester Patrick</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
         <v>1927</v>
       </c>
-      <c r="B97" t="inlineStr">
+      <c r="B98" t="inlineStr">
         <is>
           <t>Ottawa Senators</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
+      <c r="C98" t="inlineStr">
         <is>
           <t>Coach Dave Gill</t>
         </is>

</xml_diff>